<commit_message>
Added medication type extension to cerner and imdsoft slices in Medication
</commit_message>
<xml_diff>
--- a/output/nswhealthitocmedication.xlsx
+++ b/output/nswhealthitocmedication.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$87</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3049" uniqueCount="316">
   <si>
     <t>Path</t>
   </si>
@@ -1158,7 +1158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM85"/>
+  <dimension ref="A1:AM87"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -7002,7 +7002,7 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7024,14 +7024,12 @@
         <v>94</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>114</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
         <v>40</v>
@@ -7098,7 +7096,7 @@
         <v>40</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>40</v>
@@ -7109,15 +7107,17 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="B54" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>209</v>
+      </c>
       <c r="C54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F54" t="s" s="2">
         <v>49</v>
@@ -7129,29 +7129,25 @@
         <v>40</v>
       </c>
       <c r="I54" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>63</v>
+        <v>210</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>163</v>
+        <v>211</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>166</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P54" s="2"/>
       <c r="Q54" t="s" s="2">
-        <v>220</v>
+        <v>40</v>
       </c>
       <c r="R54" t="s" s="2">
         <v>40</v>
@@ -7193,36 +7189,36 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>169</v>
+        <v>40</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>170</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7230,7 +7226,7 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F55" t="s" s="2">
         <v>49</v>
@@ -7245,24 +7241,26 @@
         <v>50</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="N55" s="2"/>
+        <v>165</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>166</v>
+      </c>
       <c r="O55" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P55" s="2"/>
       <c r="Q55" t="s" s="2">
-        <v>40</v>
+        <v>220</v>
       </c>
       <c r="R55" t="s" s="2">
         <v>40</v>
@@ -7304,7 +7302,7 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7322,18 +7320,18 @@
         <v>40</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7341,7 +7339,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F56" t="s" s="2">
         <v>49</v>
@@ -7356,18 +7354,18 @@
         <v>50</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>221</v>
+        <v>172</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="M56" s="2"/>
-      <c r="N56" t="s" s="2">
-        <v>181</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
         <v>40</v>
       </c>
@@ -7415,7 +7413,7 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7433,18 +7431,18 @@
         <v>40</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7452,7 +7450,7 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F57" t="s" s="2">
         <v>49</v>
@@ -7467,17 +7465,17 @@
         <v>50</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>40</v>
@@ -7526,7 +7524,7 @@
         <v>40</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -7544,18 +7542,18 @@
         <v>40</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7578,19 +7576,17 @@
         <v>50</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>196</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="M58" s="2"/>
       <c r="N58" t="s" s="2">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>40</v>
@@ -7639,7 +7635,7 @@
         <v>40</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -7657,22 +7653,20 @@
         <v>40</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="B59" t="s" s="2">
-        <v>222</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
         <v>40</v>
       </c>
@@ -7681,7 +7675,7 @@
         <v>41</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>40</v>
@@ -7693,19 +7687,19 @@
         <v>50</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>147</v>
+        <v>193</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>40</v>
@@ -7754,13 +7748,13 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>40</v>
@@ -7772,20 +7766,22 @@
         <v>40</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>154</v>
+        <v>199</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>155</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="B60" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="B60" t="s" s="2">
+        <v>222</v>
+      </c>
       <c r="C60" t="s" s="2">
         <v>40</v>
       </c>
@@ -7794,7 +7790,7 @@
         <v>41</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>40</v>
@@ -7803,19 +7799,23 @@
         <v>40</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>137</v>
+        <v>223</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>151</v>
+      </c>
       <c r="O60" t="s" s="2">
         <v>40</v>
       </c>
@@ -7863,47 +7863,47 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>40</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>40</v>
@@ -7915,17 +7915,15 @@
         <v>40</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>114</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>40</v>
@@ -7962,31 +7960,31 @@
         <v>40</v>
       </c>
       <c r="AA61" t="s" s="2">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="AB61" t="s" s="2">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="AC61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD61" t="s" s="2">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>40</v>
@@ -8003,7 +8001,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8011,10 +8009,10 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>40</v>
@@ -8023,29 +8021,25 @@
         <v>40</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>163</v>
+        <v>95</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>166</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P62" s="2"/>
       <c r="Q62" t="s" s="2">
-        <v>224</v>
+        <v>40</v>
       </c>
       <c r="R62" t="s" s="2">
         <v>40</v>
@@ -8075,50 +8069,52 @@
         <v>40</v>
       </c>
       <c r="AA62" t="s" s="2">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="AB62" t="s" s="2">
-        <v>40</v>
+        <v>144</v>
       </c>
       <c r="AC62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD62" t="s" s="2">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>169</v>
+        <v>40</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>170</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="B63" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="B63" t="s" s="2">
+        <v>209</v>
+      </c>
       <c r="C63" t="s" s="2">
         <v>40</v>
       </c>
@@ -8136,20 +8132,18 @@
         <v>40</v>
       </c>
       <c r="I63" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>51</v>
+        <v>210</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>173</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>174</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>40</v>
@@ -8198,36 +8192,36 @@
         <v>40</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>177</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8250,24 +8244,26 @@
         <v>50</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>225</v>
+        <v>163</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="M64" s="2"/>
+        <v>164</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>165</v>
+      </c>
       <c r="N64" t="s" s="2">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>40</v>
       </c>
       <c r="P64" s="2"/>
       <c r="Q64" t="s" s="2">
-        <v>40</v>
+        <v>224</v>
       </c>
       <c r="R64" t="s" s="2">
         <v>40</v>
@@ -8309,7 +8305,7 @@
         <v>40</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -8327,18 +8323,18 @@
         <v>40</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8364,15 +8360,15 @@
         <v>51</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="M65" s="2"/>
-      <c r="N65" t="s" s="2">
-        <v>188</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>40</v>
       </c>
@@ -8420,7 +8416,7 @@
         <v>40</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8438,18 +8434,18 @@
         <v>40</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8457,7 +8453,7 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F66" t="s" s="2">
         <v>49</v>
@@ -8472,19 +8468,17 @@
         <v>50</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>193</v>
+        <v>69</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>196</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="M66" s="2"/>
       <c r="N66" t="s" s="2">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>40</v>
@@ -8533,7 +8527,7 @@
         <v>40</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
@@ -8551,18 +8545,18 @@
         <v>40</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>200</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>226</v>
+        <v>185</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8588,16 +8582,14 @@
         <v>51</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>227</v>
+        <v>186</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>229</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="M67" s="2"/>
       <c r="N67" t="s" s="2">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>40</v>
@@ -8646,7 +8638,7 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>231</v>
+        <v>189</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -8664,18 +8656,18 @@
         <v>40</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>233</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>234</v>
+        <v>192</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8692,24 +8684,26 @@
         <v>40</v>
       </c>
       <c r="H68" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I68" t="s" s="2">
         <v>50</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>69</v>
+        <v>193</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="N68" s="2"/>
+        <v>196</v>
+      </c>
+      <c r="N68" t="s" s="2">
+        <v>197</v>
+      </c>
       <c r="O68" t="s" s="2">
         <v>40</v>
       </c>
@@ -8733,13 +8727,13 @@
         <v>40</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>238</v>
+        <v>40</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>239</v>
+        <v>40</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>240</v>
+        <v>40</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>40</v>
@@ -8757,7 +8751,7 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
@@ -8775,18 +8769,18 @@
         <v>40</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>40</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8809,16 +8803,20 @@
         <v>50</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>243</v>
+        <v>51</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="N69" t="s" s="2">
+        <v>230</v>
+      </c>
       <c r="O69" t="s" s="2">
         <v>40</v>
       </c>
@@ -8866,7 +8864,7 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -8881,21 +8879,21 @@
         <v>61</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>246</v>
+        <v>40</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>248</v>
+        <v>40</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>249</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8912,22 +8910,22 @@
         <v>40</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I70" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
@@ -8953,11 +8951,13 @@
         <v>40</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="X70" s="2"/>
+        <v>238</v>
+      </c>
+      <c r="X70" t="s" s="2">
+        <v>239</v>
+      </c>
       <c r="Y70" t="s" s="2">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>40</v>
@@ -8975,7 +8975,7 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -8990,21 +8990,21 @@
         <v>61</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>255</v>
+        <v>40</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>257</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9027,13 +9027,13 @@
         <v>50</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -9084,7 +9084,7 @@
         <v>40</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
@@ -9099,21 +9099,21 @@
         <v>61</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>40</v>
+        <v>246</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>40</v>
+        <v>248</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>40</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9124,7 +9124,7 @@
         <v>41</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G72" t="s" s="2">
         <v>40</v>
@@ -9136,16 +9136,16 @@
         <v>40</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>264</v>
+        <v>125</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9171,13 +9171,11 @@
         <v>40</v>
       </c>
       <c r="W72" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="X72" s="2"/>
       <c r="Y72" t="s" s="2">
-        <v>40</v>
+        <v>254</v>
       </c>
       <c r="Z72" t="s" s="2">
         <v>40</v>
@@ -9195,13 +9193,13 @@
         <v>40</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG72" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH72" t="s" s="2">
         <v>40</v>
@@ -9210,21 +9208,21 @@
         <v>61</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>40</v>
+        <v>255</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>40</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9244,16 +9242,16 @@
         <v>40</v>
       </c>
       <c r="I73" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>51</v>
+        <v>259</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>137</v>
+        <v>260</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>138</v>
+        <v>261</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -9304,7 +9302,7 @@
         <v>40</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>139</v>
+        <v>258</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -9316,13 +9314,13 @@
         <v>40</v>
       </c>
       <c r="AI73" t="s" s="2">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="AJ73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>140</v>
+        <v>262</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>40</v>
@@ -9333,11 +9331,11 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -9356,16 +9354,16 @@
         <v>40</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>94</v>
+        <v>264</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>142</v>
+        <v>265</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>143</v>
+        <v>266</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>114</v>
+        <v>267</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
@@ -9415,7 +9413,7 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>145</v>
+        <v>263</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9427,13 +9425,13 @@
         <v>40</v>
       </c>
       <c r="AI74" t="s" s="2">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="AJ74" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>140</v>
+        <v>268</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>40</v>
@@ -9444,43 +9442,39 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>272</v>
+        <v>40</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H75" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I75" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>273</v>
+        <v>137</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
         <v>40</v>
       </c>
@@ -9528,25 +9522,25 @@
         <v>40</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>275</v>
+        <v>139</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI75" t="s" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AJ75" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>40</v>
@@ -9557,18 +9551,18 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F76" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G76" t="s" s="2">
         <v>40</v>
@@ -9580,18 +9574,18 @@
         <v>40</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>277</v>
+        <v>94</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>278</v>
+        <v>142</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="M76" s="2"/>
-      <c r="N76" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="M76" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
         <v>40</v>
       </c>
@@ -9627,81 +9621,83 @@
         <v>40</v>
       </c>
       <c r="AA76" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="AB76" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB76" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC76" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD76" t="s" s="2">
-        <v>282</v>
+        <v>40</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>276</v>
+        <v>145</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AG76" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH76" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>132</v>
+        <v>40</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>283</v>
+        <v>140</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>284</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="B77" t="s" s="2">
-        <v>285</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
-        <v>40</v>
+        <v>272</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H77" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I77" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="M77" s="2"/>
+        <v>274</v>
+      </c>
+      <c r="M77" t="s" s="2">
+        <v>114</v>
+      </c>
       <c r="N77" t="s" s="2">
-        <v>280</v>
+        <v>115</v>
       </c>
       <c r="O77" t="s" s="2">
         <v>40</v>
@@ -9726,11 +9722,13 @@
         <v>40</v>
       </c>
       <c r="W77" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="X77" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X77" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y77" t="s" s="2">
-        <v>288</v>
+        <v>40</v>
       </c>
       <c r="Z77" t="s" s="2">
         <v>40</v>
@@ -9748,36 +9746,36 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AG77" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>132</v>
+        <v>40</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>283</v>
+        <v>92</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>284</v>
+        <v>40</v>
       </c>
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9785,7 +9783,7 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F78" t="s" s="2">
         <v>49</v>
@@ -9800,17 +9798,17 @@
         <v>40</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>193</v>
+        <v>277</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" t="s" s="2">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="O78" t="s" s="2">
         <v>40</v>
@@ -9847,22 +9845,20 @@
         <v>40</v>
       </c>
       <c r="AA78" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB78" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="AB78" s="2"/>
       <c r="AC78" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD78" t="s" s="2">
-        <v>40</v>
+        <v>282</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>49</v>
@@ -9874,23 +9870,25 @@
         <v>61</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>40</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="B79" s="2"/>
+        <v>276</v>
+      </c>
+      <c r="B79" t="s" s="2">
+        <v>285</v>
+      </c>
       <c r="C79" t="s" s="2">
         <v>40</v>
       </c>
@@ -9911,16 +9909,18 @@
         <v>40</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>259</v>
+        <v>125</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
+      <c r="N79" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="O79" t="s" s="2">
         <v>40</v>
       </c>
@@ -9944,13 +9944,11 @@
         <v>40</v>
       </c>
       <c r="W79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X79" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="X79" s="2"/>
       <c r="Y79" t="s" s="2">
-        <v>40</v>
+        <v>288</v>
       </c>
       <c r="Z79" t="s" s="2">
         <v>40</v>
@@ -9968,10 +9966,10 @@
         <v>40</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>49</v>
@@ -9983,21 +9981,21 @@
         <v>61</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>297</v>
+        <v>132</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10020,16 +10018,18 @@
         <v>40</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>264</v>
+        <v>193</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
+      <c r="N80" t="s" s="2">
+        <v>292</v>
+      </c>
       <c r="O80" t="s" s="2">
         <v>40</v>
       </c>
@@ -10077,7 +10077,7 @@
         <v>40</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10092,10 +10092,10 @@
         <v>61</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>246</v>
+        <v>40</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="AL80" t="s" s="2">
         <v>40</v>
@@ -10106,7 +10106,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10129,13 +10129,13 @@
         <v>40</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>51</v>
+        <v>259</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>137</v>
+        <v>295</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>138</v>
+        <v>296</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -10186,7 +10186,7 @@
         <v>40</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>139</v>
+        <v>294</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
@@ -10198,35 +10198,35 @@
         <v>40</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>40</v>
+        <v>297</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>140</v>
+        <v>262</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>40</v>
+        <v>298</v>
       </c>
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F82" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G82" t="s" s="2">
         <v>40</v>
@@ -10238,17 +10238,15 @@
         <v>40</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>94</v>
+        <v>264</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>142</v>
+        <v>300</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>114</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" t="s" s="2">
         <v>40</v>
@@ -10297,25 +10295,25 @@
         <v>40</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>145</v>
+        <v>299</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG82" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH82" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI82" t="s" s="2">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>40</v>
+        <v>246</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>140</v>
+        <v>302</v>
       </c>
       <c r="AL82" t="s" s="2">
         <v>40</v>
@@ -10326,43 +10324,39 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>272</v>
+        <v>40</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H83" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I83" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>273</v>
+        <v>137</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="M83" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
       <c r="O83" t="s" s="2">
         <v>40</v>
       </c>
@@ -10410,25 +10404,25 @@
         <v>40</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>275</v>
+        <v>139</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI83" t="s" s="2">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AJ83" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="AL83" t="s" s="2">
         <v>40</v>
@@ -10439,18 +10433,18 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F84" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G84" t="s" s="2">
         <v>40</v>
@@ -10462,15 +10456,17 @@
         <v>40</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>307</v>
+        <v>142</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>308</v>
-      </c>
-      <c r="M84" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="M84" t="s" s="2">
+        <v>114</v>
+      </c>
       <c r="N84" s="2"/>
       <c r="O84" t="s" s="2">
         <v>40</v>
@@ -10519,68 +10515,72 @@
         <v>40</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>306</v>
+        <v>145</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG84" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="AH84" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI84" t="s" s="2">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>246</v>
+        <v>40</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>309</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
-        <v>40</v>
+        <v>272</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H85" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I85" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>311</v>
+        <v>94</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
+        <v>274</v>
+      </c>
+      <c r="M85" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="N85" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="O85" t="s" s="2">
         <v>40</v>
       </c>
@@ -10628,35 +10628,253 @@
         <v>40</v>
       </c>
       <c r="AE85" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AF85" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG85" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI85" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="AJ85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK85" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AL85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM85" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" hidden="true">
+      <c r="A86" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F86" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J86" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="K86" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="L86" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P86" s="2"/>
+      <c r="Q86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE86" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AF86" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG86" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI86" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AJ86" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="AK86" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="AL86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM86" t="s" s="2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="87" hidden="true">
+      <c r="A87" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="AF85" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG85" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI85" t="s" s="2">
+      <c r="B87" s="2"/>
+      <c r="C87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F87" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J87" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="K87" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="L87" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P87" s="2"/>
+      <c r="Q87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE87" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="AF87" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI87" t="s" s="2">
         <v>61</v>
       </c>
-      <c r="AJ85" t="s" s="2">
+      <c r="AJ87" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="AK85" t="s" s="2">
+      <c r="AK87" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="AL85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM85" t="s" s="2">
+      <c r="AL87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM87" t="s" s="2">
         <v>315</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM85">
+  <autoFilter ref="A1:AM87">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10666,7 +10884,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI84">
+  <conditionalFormatting sqref="A2:AI86">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>